<commit_message>
Small track file edits
</commit_message>
<xml_diff>
--- a/Documents/Tracks.xlsx
+++ b/Documents/Tracks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB1C041-C0E2-4910-86F6-51D6529921C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D973AD-0BE1-4C58-9A2D-859B2B5CD9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B130DD3-8182-48A3-BE71-652CC6AC2F56}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
   <si>
     <t>Chapter</t>
   </si>
@@ -315,10 +315,13 @@
     <t>FE6 Beholding Nature's Beauty</t>
   </si>
   <si>
-    <t>→ Inescapable Fate</t>
-  </si>
-  <si>
     <t>Etrian Odyssey 3 Those Who Slay and Fall</t>
+  </si>
+  <si>
+    <t>FE7 Inescapable Fate</t>
+  </si>
+  <si>
+    <t>Tracks Remaining: 12</t>
   </si>
 </sst>
 </file>
@@ -682,7 +685,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,6 +726,9 @@
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -731,6 +737,9 @@
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -740,7 +749,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -750,6 +759,9 @@
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -758,9 +770,6 @@
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -778,7 +787,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -796,9 +805,6 @@
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -909,7 +915,7 @@
         <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -956,7 +962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
@@ -964,17 +970,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>25</v>
       </c>
@@ -982,12 +988,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>27</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
@@ -1003,7 +1009,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>77</v>
       </c>
@@ -1011,27 +1017,27 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
@@ -1039,15 +1045,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>69</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
New assets and credits edits, including Slater's new portraits
</commit_message>
<xml_diff>
--- a/Documents/Tracks.xlsx
+++ b/Documents/Tracks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D973AD-0BE1-4C58-9A2D-859B2B5CD9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961B3222-50F5-4FC3-9D40-D4C8C3717E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B130DD3-8182-48A3-BE71-652CC6AC2F56}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
   <si>
     <t>Chapter</t>
   </si>
@@ -174,9 +174,6 @@
     <t>nyawenyye Crimson Ridge</t>
   </si>
   <si>
-    <t>Runa Anima Chant</t>
-  </si>
-  <si>
     <t>Ch16-C</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>Ch19-A</t>
   </si>
   <si>
-    <t>Runa Escape</t>
-  </si>
-  <si>
     <t>Ch -1</t>
   </si>
   <si>
@@ -322,6 +316,18 @@
   </si>
   <si>
     <t>Tracks Remaining: 12</t>
+  </si>
+  <si>
+    <t>Renegade Level 2</t>
+  </si>
+  <si>
+    <t>Escape (Runa)</t>
+  </si>
+  <si>
+    <t>Anima Chant (Runa)</t>
+  </si>
+  <si>
+    <t>LoZ Twilight Princess Midna's Lament</t>
   </si>
 </sst>
 </file>
@@ -685,7 +691,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -716,7 +722,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -727,7 +733,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -738,7 +744,7 @@
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -749,7 +755,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -760,7 +766,7 @@
         <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -787,7 +793,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -875,31 +881,31 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -907,15 +913,15 @@
         <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -923,20 +929,20 @@
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>38</v>
@@ -954,7 +960,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -967,12 +973,12 @@
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -985,20 +991,23 @@
         <v>25</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1006,15 +1015,15 @@
         <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1024,38 +1033,38 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>38</v>
@@ -1063,63 +1072,63 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Animations updated, new assets
</commit_message>
<xml_diff>
--- a/Documents/Tracks.xlsx
+++ b/Documents/Tracks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugob\BindingStories\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961B3222-50F5-4FC3-9D40-D4C8C3717E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414FACB8-35A4-4930-AFEF-3529FAD7A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B130DD3-8182-48A3-BE71-652CC6AC2F56}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
   <si>
     <t>Chapter</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>LoZ Twilight Princess Midna's Lament</t>
+  </si>
+  <si>
+    <t>Riviera Heaven's Gate</t>
   </si>
 </sst>
 </file>
@@ -691,7 +694,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,6 +779,9 @@
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">

</xml_diff>